<commit_message>
Added the courses dynamically(sort of :p) and updated some connectivity issues
</commit_message>
<xml_diff>
--- a/CSite/templates/Book1.xlsx
+++ b/CSite/templates/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\PycharmProjects\djangoProject\CSite\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14A2F02-D1A1-4518-B114-4D9F2C91B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298ECBDD-D0F7-4A29-8AFF-574C908DF4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B396755C-9457-4DB3-BC17-4C14CFD81F5B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="192">
   <si>
     <t>Title</t>
   </si>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E40CA80-FF18-47D8-8805-58329250DF22}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="245.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="245.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="265.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="278.39999999999998" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
@@ -1909,9 +1909,7 @@
       <c r="A39" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>188</v>
       </c>

</xml_diff>